<commit_message>
Updates to Austrian stats
</commit_message>
<xml_diff>
--- a/data/Austrian_industrial_statistics_1854.xlsx
+++ b/data/Austrian_industrial_statistics_1854.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="184">
   <si>
     <t>i . Maschinen - Flachsgarn - Spinnereien im Jahre 1854.</t>
   </si>
@@ -704,6 +704,9 @@
   </si>
   <si>
     <t>Note: Industries that are missing in Lombardy and Venetia, or are not disaggregated at the town level, are not inserted</t>
+  </si>
+  <si>
+    <t>m. Papier - Erzeugung im Jahre 1854.</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1065,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2460,7 +2463,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
@@ -2480,7 +2483,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
@@ -2501,7 +2504,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
@@ -2532,7 +2535,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
@@ -2563,7 +2566,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
@@ -2584,7 +2587,7 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
@@ -2605,7 +2608,7 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
@@ -2626,7 +2629,7 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
@@ -2647,7 +2650,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
@@ -2668,7 +2671,7 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B67" t="s">
         <v>1</v>
@@ -2688,7 +2691,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
@@ -2709,7 +2712,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
@@ -2730,7 +2733,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
@@ -2751,7 +2754,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
@@ -2772,7 +2775,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
@@ -2793,7 +2796,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
@@ -2814,7 +2817,7 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -2835,7 +2838,7 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
@@ -2856,7 +2859,7 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
@@ -2877,7 +2880,7 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
@@ -2898,7 +2901,7 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
@@ -2913,7 +2916,7 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
@@ -2934,7 +2937,7 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
@@ -2955,7 +2958,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
@@ -2976,7 +2979,7 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
@@ -2997,7 +3000,7 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
@@ -3018,7 +3021,7 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
@@ -3039,7 +3042,7 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
@@ -3060,7 +3063,7 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
@@ -3081,7 +3084,7 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
@@ -3102,7 +3105,7 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
@@ -3123,7 +3126,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
@@ -3144,7 +3147,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -3165,7 +3168,7 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B91" t="s">
         <v>1</v>
@@ -3186,7 +3189,7 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
@@ -3207,7 +3210,7 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
         <v>1</v>
@@ -3227,7 +3230,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B94" t="s">
         <v>1</v>
@@ -3247,7 +3250,7 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B95" t="s">
         <v>1</v>
@@ -3268,7 +3271,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
@@ -3289,7 +3292,7 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
@@ -3310,7 +3313,7 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
@@ -3331,7 +3334,7 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B99" t="s">
         <v>1</v>
@@ -3352,7 +3355,7 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B100" t="s">
         <v>1</v>
@@ -3373,7 +3376,7 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
@@ -3393,7 +3396,7 @@
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B102" t="s">
         <v>1</v>
@@ -3414,7 +3417,7 @@
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B103" t="s">
         <v>1</v>
@@ -3435,7 +3438,7 @@
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
@@ -3458,7 +3461,7 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
         <v>1</v>
@@ -3479,7 +3482,7 @@
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B106" t="s">
         <v>42</v>
@@ -3499,7 +3502,7 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B107" t="s">
         <v>42</v>
@@ -3519,7 +3522,7 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B108" t="s">
         <v>42</v>
@@ -3539,7 +3542,7 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B109" t="s">
         <v>42</v>
@@ -3559,7 +3562,7 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B110" t="s">
         <v>42</v>
@@ -3579,7 +3582,7 @@
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B111" t="s">
         <v>42</v>
@@ -3599,7 +3602,7 @@
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B112" t="s">
         <v>42</v>
@@ -3619,7 +3622,7 @@
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B113" t="s">
         <v>42</v>
@@ -3639,7 +3642,7 @@
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B114" t="s">
         <v>42</v>
@@ -3659,7 +3662,7 @@
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B115" t="s">
         <v>42</v>
@@ -3679,7 +3682,7 @@
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B116" t="s">
         <v>42</v>
@@ -3699,7 +3702,7 @@
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B117" t="s">
         <v>42</v>
@@ -3719,7 +3722,7 @@
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B118" t="s">
         <v>42</v>
@@ -3739,7 +3742,7 @@
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B119" t="s">
         <v>42</v>
@@ -3759,7 +3762,7 @@
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
       <c r="B120" t="s">
         <v>42</v>
@@ -4386,7 +4389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4408,20 +4411,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="849ba905-b147-4d5f-9c8c-24526156989e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="849ba905-b147-4d5f-9c8c-24526156989e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4664,26 +4667,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC72452D-8BA1-4AC9-BA43-3950A925E71C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3F9E17-51B7-4277-BC53-B62A92A491D0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="849ba905-b147-4d5f-9c8c-24526156989e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6e1ea3c6-49aa-46a0-abdd-da3db8966731"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3F9E17-51B7-4277-BC53-B62A92A491D0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC72452D-8BA1-4AC9-BA43-3950A925E71C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6e1ea3c6-49aa-46a0-abdd-da3db8966731"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="849ba905-b147-4d5f-9c8c-24526156989e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>